<commit_message>
TD et TP des messages
par : issaoui yasmine , fatima zohra sorour
</commit_message>
<xml_diff>
--- a/TDM 102 Affectation des messages.xlsx
+++ b/TDM 102 Affectation des messages.xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESSARRAJ.FOUAD\Google Drive\Formations\Modules\Programmation Structuré\Rapport_Exceptions\TDM 102\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E645292-FB39-4295-88BD-80472841F1C3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8220" xr2:uid="{7FA781EA-CE90-4B2B-B2D5-4008700FA900}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TDM 202" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TDM 202'!$A$1:$R$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
   <si>
     <t>Nom</t>
   </si>
@@ -255,12 +249,84 @@
   </si>
   <si>
     <t>RAHMA</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>Autre</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>M12</t>
+  </si>
+  <si>
+    <t>M13</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>M15</t>
+  </si>
+  <si>
+    <t>TD2</t>
+  </si>
+  <si>
+    <t>TD3</t>
+  </si>
+  <si>
+    <t>TD4</t>
+  </si>
+  <si>
+    <t>TD7</t>
+  </si>
+  <si>
+    <t>TD8</t>
+  </si>
+  <si>
+    <t>TD5</t>
+  </si>
+  <si>
+    <t>TD7.1</t>
+  </si>
+  <si>
+    <t>Pédagogie</t>
+  </si>
+  <si>
+    <t>TD14</t>
+  </si>
+  <si>
+    <t>TD16</t>
+  </si>
+  <si>
+    <t>langage C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -360,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -386,6 +452,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,17 +765,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD73496-C8EC-46B5-9F4B-13D05B006AD7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
@@ -1015,7 +1087,7 @@
       <c r="C30" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R1" xr:uid="{C66DB321-225C-47B2-93D1-0EFF9F4F9DED}">
+  <autoFilter ref="A1:R1">
     <sortState ref="A2:R29">
       <sortCondition ref="A1"/>
     </sortState>
@@ -1023,4 +1095,212 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="11.42578125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="F2" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>